<commit_message>
Added the log files and also installed the log4j2 dependency in pom file
</commit_message>
<xml_diff>
--- a/testData/doctors.xlsx
+++ b/testData/doctors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="12">
   <si>
     <t>Dr. K.A. Mohan</t>
   </si>
@@ -33,6 +33,21 @@
   </si>
   <si>
     <t>Dr. Uday Kamath</t>
+  </si>
+  <si>
+    <t>Dr. G.Chandra Sekhar</t>
+  </si>
+  <si>
+    <t>Dr. M. S. Sushma Susik</t>
+  </si>
+  <si>
+    <t>Dr. M.Manjula</t>
+  </si>
+  <si>
+    <t>Dr. S. Harinath Reddy</t>
+  </si>
+  <si>
+    <t>Dr. Surendra Kumar Alluri</t>
   </si>
 </sst>
 </file>
@@ -85,27 +100,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the grouping part
</commit_message>
<xml_diff>
--- a/testData/doctors.xlsx
+++ b/testData/doctors.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="12">
   <si>
     <t>Dr. K.A. Mohan</t>
   </si>
@@ -100,27 +100,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>